<commit_message>
Added ability for PowerPlant to run on two fuels.
Added fuel2 and efficiency2 to data files and db_schema_universal.db.

Added lines of code to temoa_model_build.py and move_data_to_universal_db.py to add fuel2 and efficiency2 to the model.

Note: Will make updates to other project data files later.
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/data/data_H2_VFB.xlsx
+++ b/projects/va_emerging_tech/data/data_H2_VFB.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70CAEF-6470-4CAD-891C-415C4D5D1D6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB65C081-CD89-4DBF-A281-C7BCAF5B3C71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="6840" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="71">
   <si>
     <t>connection</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>CapacityCreditIncr</t>
+  </si>
+  <si>
+    <t>fuel2</t>
+  </si>
+  <si>
+    <t>Efficiency2</t>
   </si>
 </sst>
 </file>
@@ -576,25 +582,25 @@
       <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.07421875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.4609375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.4609375" customWidth="1"/>
+    <col min="15" max="15" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.07421875" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +656,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -720,25 +726,25 @@
       <selection activeCell="R1" sqref="R1:S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.69140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.07421875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.07421875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -797,7 +803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -856,7 +862,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -873,7 +879,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -890,7 +896,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -907,7 +913,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -924,7 +930,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -941,7 +947,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -966,22 +972,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3046875" customWidth="1"/>
+    <col min="4" max="4" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -989,34 +996,37 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
@@ -1027,7 +1037,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>45</v>
@@ -1041,13 +1051,16 @@
       <c r="H2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1059,24 +1072,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.69140625" customWidth="1"/>
+    <col min="6" max="6" width="12.765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1090,22 +1104,25 @@
         <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
@@ -1119,18 +1136,21 @@
         <v>38</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="H2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1148,23 +1168,23 @@
       <selection activeCell="A3" sqref="A3:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.07421875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" customWidth="1"/>
+    <col min="13" max="13" width="9.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -1202,7 +1222,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1254,20 +1274,20 @@
       <selection activeCell="A3" sqref="A3:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1299,7 +1319,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>34</v>
       </c>

</xml_diff>